<commit_message>
Feature delta statistics until Sept 18
</commit_message>
<xml_diff>
--- a/statistics/DeltaJavaTeamprojectStatistics.xlsx
+++ b/statistics/DeltaJavaTeamprojectStatistics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\SPLTeamprojektMigrated\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1BA97D-6710-4C94-A2B5-E7D7718900B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A000278C-6E75-4070-9CFE-9A345096C6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{49590200-070D-493A-A4E6-BC83A69EFD86}"/>
   </bookViews>
@@ -712,7 +712,7 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added summed up values and improved diagrams
</commit_message>
<xml_diff>
--- a/statistics/DeltaJavaTeamprojectStatistics.xlsx
+++ b/statistics/DeltaJavaTeamprojectStatistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\repositories\ProjectSPLDevelopment\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF4497F-B4BE-4226-8175-0A08113711CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CBDD1A-DE65-4AB3-9067-D553C26F78DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1275" yWindow="-120" windowWidth="37245" windowHeight="21840" xr2:uid="{49590200-070D-493A-A4E6-BC83A69EFD86}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <author>tc={DE2886DC-191F-4616-91D6-2495B51F4D30}</author>
   </authors>
   <commentList>
-    <comment ref="A45" authorId="0" shapeId="0" xr:uid="{DE2886DC-191F-4616-91D6-2495B51F4D30}">
+    <comment ref="A46" authorId="0" shapeId="0" xr:uid="{DE2886DC-191F-4616-91D6-2495B51F4D30}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="111">
   <si>
     <t>#Adds</t>
   </si>
@@ -378,14 +378,20 @@
     <t>Average (feature interaction deltas)</t>
   </si>
   <si>
-    <t>Average ("normal" deltas)</t>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Sume</t>
+  </si>
+  <si>
+    <t>Average (feature deltas)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,12 +406,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -751,7 +751,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A45" dT="2021-06-30T11:29:33.75" personId="{D7A62C97-611E-4BD1-AF2A-25A73D55135F}" id="{DE2886DC-191F-4616-91D6-2495B51F4D30}">
+  <threadedComment ref="A46" dT="2021-06-30T11:29:33.75" personId="{D7A62C97-611E-4BD1-AF2A-25A73D55135F}" id="{DE2886DC-191F-4616-91D6-2495B51F4D30}">
     <text>is also a code sharing delta. Not entirely clear why this is not necessary for TravelTime || RemainingTravelTime.</text>
   </threadedComment>
 </ThreadedComments>
@@ -759,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAC55B7-25C4-446C-8A63-DB5C52D417FB}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B37"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1641,7 +1641,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C38">
         <f>AVERAGE(C2:C37)</f>
@@ -1664,40 +1664,42 @@
         <v>12.333333333333334</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39">
+        <f>SUM(C2:C37)</f>
+        <v>3891</v>
+      </c>
+      <c r="D39">
+        <f t="shared" ref="D39:G39" si="1">SUM(D2:D37)</f>
+        <v>341</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>444</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>90</v>
-      </c>
-      <c r="B41" t="s">
-        <v>19</v>
-      </c>
-      <c r="C41">
-        <v>13</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>2</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="C42">
         <v>13</v>
@@ -1717,10 +1719,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C43">
         <v>13</v>
@@ -1740,10 +1742,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C44">
         <v>13</v>
@@ -1763,16 +1765,16 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C45">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -1781,24 +1783,21 @@
         <v>0</v>
       </c>
       <c r="G45">
-        <v>4</v>
-      </c>
-      <c r="I45" t="s">
-        <v>101</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B46" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C46">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E46">
         <v>2</v>
@@ -1807,15 +1806,18 @@
         <v>0</v>
       </c>
       <c r="G46">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="I46" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C47">
         <v>13</v>
@@ -1835,133 +1837,206 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C48">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="D48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48">
         <v>0</v>
       </c>
       <c r="G48">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49">
+        <v>43</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>107</v>
       </c>
-      <c r="C49">
-        <f>AVERAGE(C41:C48)</f>
+      <c r="C50">
+        <f>AVERAGE(C42:C49)</f>
         <v>21</v>
       </c>
-      <c r="D49">
-        <f t="shared" ref="D49:G49" si="1">AVERAGE(D41:D48)</f>
+      <c r="D50">
+        <f t="shared" ref="D50:G50" si="2">AVERAGE(D42:D49)</f>
         <v>0.5</v>
       </c>
-      <c r="E49">
-        <f t="shared" si="1"/>
+      <c r="E50">
+        <f t="shared" si="2"/>
         <v>2.125</v>
       </c>
-      <c r="F49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G49">
-        <f t="shared" si="1"/>
+      <c r="F50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="2"/>
         <v>2.625</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51">
+        <f>SUM(C42:C49)</f>
+        <v>168</v>
+      </c>
+      <c r="D51">
+        <f t="shared" ref="D51:G51" si="3">SUM(D42:D49)</f>
+        <v>4</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>5</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
         <v>8</v>
       </c>
-      <c r="C52">
+      <c r="C54">
         <v>41</v>
       </c>
-      <c r="D52">
+      <c r="D54">
         <v>6</v>
       </c>
-      <c r="E52">
-        <v>2</v>
-      </c>
-      <c r="F52">
-        <v>0</v>
-      </c>
-      <c r="G52">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>106</v>
-      </c>
-      <c r="C53">
-        <f>AVERAGE(C52:C52)</f>
-        <v>41</v>
-      </c>
-      <c r="D53">
-        <f>AVERAGE(D52:D52)</f>
-        <v>6</v>
-      </c>
-      <c r="E53">
-        <f>AVERAGE(E52:E52)</f>
-        <v>2</v>
-      </c>
-      <c r="F53">
-        <f>AVERAGE(F52:F52)</f>
-        <v>0</v>
-      </c>
-      <c r="G53">
-        <f>AVERAGE(G52:G52)</f>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
         <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55">
+        <f>AVERAGE(C54:C54)</f>
+        <v>41</v>
+      </c>
+      <c r="D55">
+        <f>AVERAGE(D54:D54)</f>
+        <v>6</v>
+      </c>
+      <c r="E55">
+        <f>AVERAGE(E54:E54)</f>
+        <v>2</v>
+      </c>
+      <c r="F55">
+        <f>AVERAGE(F54:F54)</f>
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <f>AVERAGE(G54:G54)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>105</v>
       </c>
-      <c r="C55">
-        <f>AVERAGE(C2:C37,C41:C48,C52:C52)</f>
+      <c r="C57">
+        <f>AVERAGE(C2:C37,C42:C49,C54:C54)</f>
         <v>91.111111111111114</v>
       </c>
-      <c r="D55">
-        <f t="shared" ref="D55:G55" si="2">AVERAGE(D2:D37,D41:D48,D52:D52)</f>
+      <c r="D57">
+        <f t="shared" ref="D57:G57" si="4">AVERAGE(D2:D37,D42:D49,D54:D54)</f>
         <v>7.8</v>
       </c>
-      <c r="E55">
-        <f t="shared" si="2"/>
+      <c r="E57">
+        <f t="shared" si="4"/>
         <v>2.7111111111111112</v>
       </c>
-      <c r="F55">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G55">
-        <f t="shared" si="2"/>
+      <c r="F57">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="4"/>
         <v>10.511111111111111</v>
       </c>
     </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>108</v>
+      </c>
+      <c r="C58">
+        <f>SUM(C2:C37,C42:C49,C54)</f>
+        <v>4100</v>
+      </c>
+      <c r="D58">
+        <f t="shared" ref="D58:G58" si="5">SUM(D2:D37,D42:D49,D54)</f>
+        <v>351</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="5"/>
+        <v>122</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="5"/>
+        <v>473</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G47">
-    <sortCondition ref="B1:B47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G48">
+    <sortCondition ref="B1:B48"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>